<commit_message>
Add Section model import and handle section retrieval in alumni_import; update error handling in footer email submission; modify user is_active field default value in migrations
</commit_message>
<xml_diff>
--- a/static/templates/alumni_import_template.xlsx
+++ b/static/templates/alumni_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guian\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C83F538-8EB1-41F5-B963-FAB686EDBC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDB58A0-AC35-44FF-9614-931708089BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21336" windowHeight="11376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>First Name</t>
   </si>
@@ -191,9 +191,6 @@
     <t>School Year</t>
   </si>
   <si>
-    <t>2016-2017</t>
-  </si>
-  <si>
     <t>Juan</t>
   </si>
   <si>
@@ -206,10 +203,25 @@
     <t>0000-00000-MN-0</t>
   </si>
   <si>
-    <t>sample_email@gmail.com</t>
-  </si>
-  <si>
     <t>639000000000</t>
+  </si>
+  <si>
+    <t>2023-2024</t>
+  </si>
+  <si>
+    <t>BSCPE</t>
+  </si>
+  <si>
+    <t>Bachelor's of Science in Computer Engineering</t>
+  </si>
+  <si>
+    <t>sample_aemail@gmail.com</t>
+  </si>
+  <si>
+    <t>Section Code</t>
+  </si>
+  <si>
+    <t>3P</t>
   </si>
 </sst>
 </file>
@@ -219,7 +231,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +248,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -288,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -306,6 +324,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -609,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:Q92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,16 +645,17 @@
     <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="67.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="67.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,45 +690,48 @@
         <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G2" s="3">
         <v>32825</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
@@ -717,101 +740,294 @@
         <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="L2" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="M2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
         <v>53</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="7">
+      <c r="Q2" s="7">
         <v>45762</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F3" s="6"/>
-      <c r="P3" s="7"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F4" s="6"/>
-      <c r="P4" s="7"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F5" s="6"/>
-      <c r="P5" s="7"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F6" s="6"/>
-      <c r="P6" s="7"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F7" s="6"/>
-      <c r="P7" s="7"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F8" s="6"/>
-      <c r="P8" s="7"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F9" s="6"/>
-      <c r="P9" s="7"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F10" s="6"/>
-      <c r="P10" s="7"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F11" s="6"/>
-      <c r="P11" s="7"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F12" s="6"/>
-      <c r="P12" s="7"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F13" s="6"/>
-      <c r="P13" s="7"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F14" s="6"/>
-      <c r="P14" s="7"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F15" s="6"/>
-      <c r="P15" s="7"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F16" s="6"/>
-      <c r="P16" s="7"/>
-    </row>
-    <row r="17" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F17" s="6"/>
-      <c r="P17" s="7"/>
-    </row>
-    <row r="18" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F18" s="6"/>
-      <c r="P18" s="7"/>
-    </row>
-    <row r="19" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F19" s="6"/>
-      <c r="P19" s="7"/>
-    </row>
-    <row r="20" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F20" s="6"/>
-      <c r="P20" s="7"/>
-    </row>
-    <row r="21" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F21" s="6"/>
-      <c r="P21" s="7"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F3" s="9"/>
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H8"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H10"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H39"/>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H40"/>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H41"/>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H42"/>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H43"/>
+    </row>
+    <row r="44" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H44"/>
+    </row>
+    <row r="45" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H45"/>
+    </row>
+    <row r="46" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H46"/>
+    </row>
+    <row r="47" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H47"/>
+    </row>
+    <row r="48" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H48"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H49"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H50"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H51"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H52"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H53"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H54"/>
+    </row>
+    <row r="55" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H55"/>
+    </row>
+    <row r="56" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H56"/>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H57"/>
+    </row>
+    <row r="58" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H58"/>
+    </row>
+    <row r="59" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H59"/>
+    </row>
+    <row r="60" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H60"/>
+    </row>
+    <row r="61" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H61"/>
+    </row>
+    <row r="62" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H62"/>
+    </row>
+    <row r="63" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H63"/>
+    </row>
+    <row r="64" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H64"/>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H65"/>
+    </row>
+    <row r="66" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H66"/>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H67"/>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H68"/>
+    </row>
+    <row r="69" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H69"/>
+    </row>
+    <row r="70" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H70"/>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H71"/>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H72"/>
+    </row>
+    <row r="73" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H73"/>
+    </row>
+    <row r="74" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H74"/>
+    </row>
+    <row r="75" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H75"/>
+    </row>
+    <row r="76" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H76"/>
+    </row>
+    <row r="77" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H77"/>
+    </row>
+    <row r="78" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H78"/>
+    </row>
+    <row r="79" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H79"/>
+    </row>
+    <row r="80" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H80"/>
+    </row>
+    <row r="81" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H81"/>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H82"/>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H83"/>
+    </row>
+    <row r="84" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H84"/>
+    </row>
+    <row r="85" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H85"/>
+    </row>
+    <row r="86" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H86"/>
+    </row>
+    <row r="87" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H87"/>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H88"/>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H89"/>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H90"/>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H91"/>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H92"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{005595E0-A1AA-497C-9F47-E3541D813FE0}"/>
   </hyperlinks>

</xml_diff>